<commit_message>
B7 , SIT bug fixes
</commit_message>
<xml_diff>
--- a/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormB7.xlsx
+++ b/RAMS/Web/RAMMS.Web.UI/wwwroot/Templates/FormB7.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>CODE</t>
   </si>
@@ -52,9 +52,6 @@
   <si>
     <t/>
   </si>
-  <si>
-    <t>MATERIALS</t>
-  </si>
 </sst>
 </file>
 
@@ -64,7 +61,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,11 +107,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -196,7 +188,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,21 +229,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -263,9 +262,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,7 +553,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,59 +571,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="25"/>
+      <c r="G2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="22"/>
+      <c r="K2" s="25"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="24"/>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
@@ -640,7 +636,7 @@
       <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="6"/>
+      <c r="E4" s="5"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
       <c r="I4" s="3"/>
@@ -652,7 +648,7 @@
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
       <c r="G5" s="3"/>
       <c r="H5" s="4"/>
       <c r="I5" s="3"/>
@@ -664,7 +660,7 @@
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="5"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
       <c r="I6" s="7"/>
@@ -676,7 +672,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="5"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
       <c r="I7" s="7"/>
@@ -688,7 +684,7 @@
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="E8" s="5"/>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
       <c r="I8" s="7"/>
@@ -700,7 +696,7 @@
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
+      <c r="E9" s="5"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="7"/>
@@ -712,7 +708,7 @@
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
+      <c r="E10" s="5"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="7"/>
@@ -724,7 +720,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
+      <c r="E11" s="5"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
       <c r="I11" s="7"/>
@@ -732,6 +728,7 @@
       <c r="K11" s="10"/>
     </row>
     <row r="12" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="16"/>
       <c r="F12" t="s">
         <v>7</v>
       </c>
@@ -742,19 +739,11 @@
       <c r="K12" s="10"/>
     </row>
     <row r="13" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="22"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
       <c r="I13" s="7"/>
@@ -762,15 +751,11 @@
       <c r="K13" s="10"/>
     </row>
     <row r="14" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
       <c r="I14" s="7"/>
@@ -781,8 +766,8 @@
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="12"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="15"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
       <c r="I15" s="7"/>
@@ -793,8 +778,8 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
       <c r="I16" s="7"/>
@@ -805,8 +790,8 @@
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
       <c r="I17" s="7"/>
@@ -817,8 +802,8 @@
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
       <c r="I18" s="7"/>
@@ -829,8 +814,8 @@
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
@@ -841,8 +826,8 @@
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="10"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
       <c r="I20" s="7"/>
@@ -853,8 +838,8 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
       <c r="I21" s="7"/>
@@ -865,8 +850,8 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="10"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
       <c r="I22" s="7"/>
@@ -877,8 +862,8 @@
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
       <c r="I23" s="7"/>
@@ -889,8 +874,8 @@
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="10"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
       <c r="G24" s="7"/>
       <c r="H24" s="8"/>
       <c r="I24" s="7"/>
@@ -901,8 +886,8 @@
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="10"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
       <c r="I25" s="7"/>
@@ -913,8 +898,8 @@
       <c r="A26" s="7"/>
       <c r="B26" s="8"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="10"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
       <c r="G26" s="7"/>
       <c r="H26" s="8"/>
       <c r="I26" s="7"/>
@@ -925,8 +910,8 @@
       <c r="A27" s="7"/>
       <c r="B27" s="8"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
       <c r="G27" s="7"/>
       <c r="H27" s="8"/>
       <c r="I27" s="7"/>
@@ -937,8 +922,8 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="7"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
       <c r="G28" s="7"/>
       <c r="H28" s="8"/>
       <c r="I28" s="7"/>
@@ -949,8 +934,8 @@
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
       <c r="I29" s="7"/>
@@ -961,8 +946,8 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
       <c r="I30" s="7"/>
@@ -973,8 +958,8 @@
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="10"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
       <c r="G31" s="7"/>
       <c r="H31" s="8"/>
       <c r="I31" s="7"/>
@@ -985,8 +970,8 @@
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="10"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
       <c r="G32" s="7"/>
       <c r="H32" s="8"/>
       <c r="I32" s="7"/>
@@ -997,8 +982,8 @@
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="10"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
       <c r="G33" s="7"/>
       <c r="H33" s="8"/>
       <c r="I33" s="7"/>
@@ -1009,8 +994,8 @@
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
       <c r="G34" s="7"/>
       <c r="H34" s="8"/>
       <c r="I34" s="7"/>
@@ -1021,8 +1006,8 @@
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="10"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
       <c r="G35" s="7"/>
       <c r="H35" s="8"/>
       <c r="I35" s="7"/>
@@ -1033,8 +1018,8 @@
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
       <c r="G36" s="7"/>
       <c r="H36" s="8"/>
       <c r="I36" s="7"/>
@@ -1045,8 +1030,8 @@
       <c r="A37" s="7"/>
       <c r="B37" s="8"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="10"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
       <c r="G37" s="7"/>
       <c r="H37" s="8"/>
       <c r="I37" s="7"/>
@@ -1057,8 +1042,8 @@
       <c r="A38" s="7"/>
       <c r="B38" s="8"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="10"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
       <c r="G38" s="7"/>
       <c r="H38" s="8"/>
       <c r="I38" s="7"/>
@@ -1069,8 +1054,8 @@
       <c r="A39" s="7"/>
       <c r="B39" s="8"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
       <c r="G39" s="7"/>
       <c r="H39" s="8"/>
       <c r="I39" s="7"/>
@@ -1078,6 +1063,11 @@
       <c r="K39" s="10"/>
     </row>
     <row r="40" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
       <c r="G40" s="7"/>
       <c r="H40" s="8"/>
       <c r="I40" s="7"/>
@@ -1085,6 +1075,11 @@
       <c r="K40" s="10"/>
     </row>
     <row r="41" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
       <c r="G41" s="7"/>
       <c r="H41" s="8"/>
       <c r="I41" s="7"/>
@@ -1092,6 +1087,11 @@
       <c r="K41" s="10"/>
     </row>
     <row r="42" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
       <c r="G42" s="7"/>
       <c r="H42" s="8"/>
       <c r="I42" s="7"/>
@@ -1099,6 +1099,11 @@
       <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
       <c r="G43" s="7"/>
       <c r="H43" s="8"/>
       <c r="I43" s="7"/>
@@ -1106,6 +1111,11 @@
       <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
       <c r="G44" s="7"/>
       <c r="H44" s="8"/>
       <c r="I44" s="7"/>
@@ -1113,6 +1123,11 @@
       <c r="K44" s="10"/>
     </row>
     <row r="45" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
       <c r="G45" s="7"/>
       <c r="H45" s="8"/>
       <c r="I45" s="7"/>
@@ -1120,6 +1135,11 @@
       <c r="K45" s="10"/>
     </row>
     <row r="46" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
       <c r="G46" s="7"/>
       <c r="H46" s="8"/>
       <c r="I46" s="7"/>
@@ -1127,6 +1147,11 @@
       <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
       <c r="G47" s="7"/>
       <c r="H47" s="8"/>
       <c r="I47" s="7"/>
@@ -1134,6 +1159,11 @@
       <c r="K47" s="10"/>
     </row>
     <row r="48" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
       <c r="G48" s="7"/>
       <c r="H48" s="8"/>
       <c r="I48" s="7"/>
@@ -1141,6 +1171,11 @@
       <c r="K48" s="10"/>
     </row>
     <row r="49" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
       <c r="G49" s="7"/>
       <c r="H49" s="8"/>
       <c r="I49" s="7"/>
@@ -1148,6 +1183,11 @@
       <c r="K49" s="10"/>
     </row>
     <row r="50" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
       <c r="G50" s="7"/>
       <c r="H50" s="8"/>
       <c r="I50" s="7"/>
@@ -1155,32 +1195,33 @@
       <c r="K50" s="10"/>
     </row>
     <row r="51" spans="1:11" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
       <c r="G51" s="7"/>
       <c r="H51" s="8"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
-      <c r="K51" s="16"/>
+      <c r="K51" s="20"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="17"/>
+      <c r="A52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="17"/>
+      <c r="A53" s="14"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="15"/>
+      <c r="D53" s="15"/>
+      <c r="E53" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:E13"/>
+  <mergeCells count="9">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>

</xml_diff>